<commit_message>
Updated CIWD 3.0 status for allele resolution
</commit_message>
<xml_diff>
--- a/reference_alleles/generate_references/CWD.Data/Reference.CWD.Status.xlsx
+++ b/reference_alleles/generate_references/CWD.Data/Reference.CWD.Status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Supplemental 1A. Ref Sequence Lists" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Supplemental 1A. Ref Sequence L" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Supplemental 1B. Refs Per Locus" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Supplemental 1C. Ref CWD Status" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9055" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9055" uniqueCount="580">
   <si>
     <t xml:space="preserve">3.25.0 Allele Name</t>
   </si>
@@ -1708,7 +1708,7 @@
 Loci:HLA-A,-B,-C,-DRB1,-DRB3,-DRB4,-DRB5,-DQA1,-DQB1,-DPA1,-DPB1</t>
   </si>
   <si>
-    <t xml:space="preserve">CWD 3.0
+    <t xml:space="preserve">CIWD 3.0
 https://doi.org/10.1111/tan.13811
 Loci:HLA-A,-B,-C,-DRB1,-DRB3,-DRB4,-DRB5,-DQB1,-DPB1</t>
   </si>
@@ -1759,6 +1759,9 @@
   </si>
   <si>
     <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not CIWD defined</t>
   </si>
   <si>
     <t xml:space="preserve">HLA-B*56:01:01:01</t>
@@ -1781,7 +1784,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1828,7 +1831,12 @@
     <font>
       <b val="true"/>
       <sz val="8"/>
-      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
@@ -1889,7 +1897,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1950,7 +1958,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2049,7 +2061,7 @@
   </sheetPr>
   <dimension ref="A1:CK128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
@@ -31510,19 +31522,24 @@
   </sheetPr>
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="25.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="50.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="55.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31552,22 +31569,22 @@
       <c r="A2" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31575,22 +31592,22 @@
       <c r="A3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31598,22 +31615,22 @@
       <c r="A4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31621,22 +31638,22 @@
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31644,22 +31661,22 @@
       <c r="A6" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31667,22 +31684,22 @@
       <c r="A7" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31690,22 +31707,22 @@
       <c r="A8" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -31713,22 +31730,22 @@
       <c r="A9" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31736,22 +31753,22 @@
       <c r="A10" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31759,22 +31776,22 @@
       <c r="A11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31782,22 +31799,22 @@
       <c r="A12" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31805,22 +31822,22 @@
       <c r="A13" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31828,22 +31845,22 @@
       <c r="A14" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31851,22 +31868,22 @@
       <c r="A15" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -31874,22 +31891,22 @@
       <c r="A16" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -31897,22 +31914,22 @@
       <c r="A17" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -31920,22 +31937,22 @@
       <c r="A18" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -31943,22 +31960,22 @@
       <c r="A19" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31966,22 +31983,22 @@
       <c r="A20" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E20" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -31989,22 +32006,22 @@
       <c r="A21" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32012,22 +32029,22 @@
       <c r="A22" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32035,22 +32052,22 @@
       <c r="A23" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -32058,22 +32075,22 @@
       <c r="A24" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32081,22 +32098,22 @@
       <c r="A25" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32104,22 +32121,22 @@
       <c r="A26" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G26" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32127,22 +32144,22 @@
       <c r="A27" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32150,22 +32167,22 @@
       <c r="A28" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32173,22 +32190,22 @@
       <c r="A29" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G29" s="15" t="s">
+      <c r="G29" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32196,22 +32213,22 @@
       <c r="A30" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32219,22 +32236,22 @@
       <c r="A31" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G31" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32242,22 +32259,22 @@
       <c r="A32" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G32" s="15" t="s">
+      <c r="G32" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32265,22 +32282,22 @@
       <c r="A33" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F33" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G33" s="15" t="s">
+      <c r="G33" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32288,22 +32305,22 @@
       <c r="A34" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D34" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E34" s="15" t="s">
+      <c r="D34" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32311,22 +32328,22 @@
       <c r="A35" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G35" s="15" t="s">
+      <c r="G35" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32334,22 +32351,22 @@
       <c r="A36" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D36" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="D36" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E36" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G36" s="15" t="s">
+      <c r="G36" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32357,22 +32374,22 @@
       <c r="A37" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G37" s="15" t="s">
+      <c r="G37" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32380,22 +32397,22 @@
       <c r="A38" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E38" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="F38" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F38" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G38" s="15" t="s">
+      <c r="G38" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -32403,22 +32420,22 @@
       <c r="A39" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G39" s="15" t="s">
+      <c r="G39" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32426,22 +32443,22 @@
       <c r="A40" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G40" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32449,22 +32466,22 @@
       <c r="A41" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G41" s="15" t="s">
+      <c r="G41" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32472,22 +32489,22 @@
       <c r="A42" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D42" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E42" s="15" t="s">
+      <c r="D42" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E42" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G42" s="15" t="s">
+      <c r="G42" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32495,22 +32512,22 @@
       <c r="A43" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E43" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G43" s="15" t="s">
+      <c r="G43" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32518,22 +32535,22 @@
       <c r="A44" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G44" s="15" t="s">
+      <c r="G44" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32541,22 +32558,22 @@
       <c r="A45" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E45" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G45" s="15" t="s">
+      <c r="G45" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32564,22 +32581,22 @@
       <c r="A46" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G46" s="15" t="s">
+      <c r="G46" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32587,22 +32604,22 @@
       <c r="A47" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G47" s="15" t="s">
+      <c r="G47" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32610,22 +32627,22 @@
       <c r="A48" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G48" s="15" t="s">
+      <c r="G48" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32633,22 +32650,22 @@
       <c r="A49" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G49" s="15" t="s">
+      <c r="G49" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32656,22 +32673,22 @@
       <c r="A50" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G50" s="15" t="s">
+      <c r="G50" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32679,22 +32696,22 @@
       <c r="A51" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D51" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="E51" s="15" t="s">
+      <c r="D51" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E51" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G51" s="15" t="s">
+      <c r="G51" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32702,45 +32719,45 @@
       <c r="A52" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="16" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>575</v>
-      </c>
-      <c r="B53" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B53" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G53" s="15" t="s">
+      <c r="G53" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32748,22 +32765,22 @@
       <c r="A54" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D54" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E54" s="15" t="s">
+      <c r="D54" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E54" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G54" s="15" t="s">
+      <c r="G54" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32771,22 +32788,22 @@
       <c r="A55" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F55" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E55" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G55" s="15" t="s">
+      <c r="G55" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32794,22 +32811,22 @@
       <c r="A56" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D56" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E56" s="15" t="s">
+      <c r="D56" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G56" s="15" t="s">
+      <c r="G56" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32817,22 +32834,22 @@
       <c r="A57" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E57" s="15" t="s">
+      <c r="D57" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F57" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="G57" s="15" t="s">
+      <c r="G57" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32840,22 +32857,22 @@
       <c r="A58" s="12" t="s">
         <v>228</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D58" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E58" s="15" t="s">
+      <c r="D58" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E58" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G58" s="15" t="s">
+      <c r="G58" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -32863,22 +32880,22 @@
       <c r="A59" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E59" s="15" t="s">
+      <c r="E59" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F59" s="15" t="s">
+      <c r="F59" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G59" s="15" t="s">
+      <c r="G59" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32886,22 +32903,22 @@
       <c r="A60" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E60" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="F60" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G60" s="15" t="s">
+      <c r="G60" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32909,22 +32926,22 @@
       <c r="A61" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F61" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G61" s="15" t="s">
+      <c r="G61" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -32932,22 +32949,22 @@
       <c r="A62" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F62" s="16" t="s">
         <v>573</v>
       </c>
-      <c r="G62" s="15" t="s">
+      <c r="G62" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -32955,22 +32972,22 @@
       <c r="A63" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="E63" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F63" s="15" t="s">
-        <v>576</v>
-      </c>
-      <c r="G63" s="15" t="s">
+      <c r="F63" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="G63" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -32978,22 +32995,22 @@
       <c r="A64" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E64" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F64" s="15" t="s">
+      <c r="F64" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G64" s="15" t="s">
+      <c r="G64" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33001,22 +33018,22 @@
       <c r="A65" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F65" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G65" s="15" t="s">
+      <c r="G65" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33024,22 +33041,22 @@
       <c r="A66" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D66" s="15" t="s">
+      <c r="C66" s="15" t="s">
+        <v>578</v>
+      </c>
+      <c r="D66" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F66" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G66" s="15" t="s">
+      <c r="G66" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33047,22 +33064,22 @@
       <c r="A67" s="12" t="s">
         <v>268</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E67" s="15" t="s">
+      <c r="E67" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F67" s="15" t="s">
+      <c r="F67" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G67" s="15" t="s">
+      <c r="G67" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33070,22 +33087,22 @@
       <c r="A68" s="12" t="s">
         <v>275</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D68" s="15" t="s">
+      <c r="D68" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E68" s="15" t="s">
+      <c r="E68" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F68" s="15" t="s">
+      <c r="F68" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="G68" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33093,22 +33110,22 @@
       <c r="A69" s="12" t="s">
         <v>278</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C69" s="1" t="s">
+      <c r="C69" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D69" s="15" t="s">
+      <c r="D69" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E69" s="15" t="s">
+      <c r="E69" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F69" s="15" t="s">
+      <c r="F69" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G69" s="15" t="s">
+      <c r="G69" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33116,22 +33133,22 @@
       <c r="A70" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D70" s="15" t="s">
+      <c r="D70" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E70" s="15" t="s">
+      <c r="E70" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F70" s="15" t="s">
+      <c r="F70" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G70" s="15" t="s">
+      <c r="G70" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33139,22 +33156,22 @@
       <c r="A71" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C71" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D71" s="15" t="s">
+      <c r="D71" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E71" s="15" t="s">
+      <c r="E71" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F71" s="15" t="s">
+      <c r="F71" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G71" s="15" t="s">
+      <c r="G71" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33162,22 +33179,22 @@
       <c r="A72" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D72" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="E72" s="15" t="s">
+      <c r="D72" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E72" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F72" s="15" t="s">
+      <c r="F72" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G72" s="15" t="s">
+      <c r="G72" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33185,22 +33202,22 @@
       <c r="A73" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D73" s="15" t="s">
+      <c r="D73" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F73" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E73" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F73" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G73" s="15" t="s">
+      <c r="G73" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33208,22 +33225,22 @@
       <c r="A74" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D74" s="15" t="s">
+      <c r="D74" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E74" s="15" t="s">
+      <c r="E74" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F74" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33231,22 +33248,22 @@
       <c r="A75" s="12" t="s">
         <v>298</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C75" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D75" s="15" t="s">
+      <c r="D75" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E75" s="15" t="s">
+      <c r="E75" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F75" s="15" t="s">
+      <c r="F75" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G75" s="15" t="s">
+      <c r="G75" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33254,22 +33271,22 @@
       <c r="A76" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="C76" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D76" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F76" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E76" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G76" s="15" t="s">
+      <c r="G76" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -33277,22 +33294,22 @@
       <c r="A77" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C77" s="1" t="s">
+      <c r="C77" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E77" s="15" t="s">
+      <c r="E77" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F77" s="15" t="s">
+      <c r="F77" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G77" s="15" t="s">
+      <c r="G77" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33300,22 +33317,22 @@
       <c r="A78" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C78" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D78" s="15" t="s">
+      <c r="D78" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E78" s="15" t="s">
+      <c r="E78" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F78" s="15" t="s">
+      <c r="F78" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G78" s="15" t="s">
+      <c r="G78" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33323,22 +33340,22 @@
       <c r="A79" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C79" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E79" s="15" t="s">
+      <c r="E79" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F79" s="15" t="s">
+      <c r="F79" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G79" s="15" t="s">
+      <c r="G79" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33346,22 +33363,22 @@
       <c r="A80" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C80" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E80" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E80" s="15" t="s">
+      <c r="F80" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F80" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G80" s="15" t="s">
+      <c r="G80" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33369,22 +33386,22 @@
       <c r="A81" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C81" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E81" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E81" s="15" t="s">
+      <c r="F81" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F81" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G81" s="15" t="s">
+      <c r="G81" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33392,22 +33409,22 @@
       <c r="A82" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="C82" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="D82" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E82" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E82" s="15" t="s">
+      <c r="F82" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F82" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G82" s="15" t="s">
+      <c r="G82" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33415,22 +33432,22 @@
       <c r="A83" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C83" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E83" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E83" s="15" t="s">
+      <c r="F83" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F83" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G83" s="15" t="s">
+      <c r="G83" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33438,22 +33455,22 @@
       <c r="A84" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C84" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E84" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E84" s="15" t="s">
+      <c r="F84" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F84" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G84" s="15" t="s">
+      <c r="G84" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33461,22 +33478,22 @@
       <c r="A85" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C85" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E85" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E85" s="15" t="s">
+      <c r="F85" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F85" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G85" s="15" t="s">
+      <c r="G85" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33484,22 +33501,22 @@
       <c r="A86" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C86" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E86" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E86" s="15" t="s">
+      <c r="F86" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F86" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G86" s="15" t="s">
+      <c r="G86" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33507,22 +33524,22 @@
       <c r="A87" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E87" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E87" s="15" t="s">
+      <c r="F87" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F87" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G87" s="15" t="s">
+      <c r="G87" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33530,22 +33547,22 @@
       <c r="A88" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C88" s="1" t="s">
+      <c r="C88" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="D88" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E88" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E88" s="15" t="s">
+      <c r="F88" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F88" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G88" s="15" t="s">
+      <c r="G88" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33553,22 +33570,22 @@
       <c r="A89" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C89" s="1" t="s">
+      <c r="C89" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D89" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E89" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E89" s="15" t="s">
+      <c r="F89" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F89" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G89" s="15" t="s">
+      <c r="G89" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33576,22 +33593,22 @@
       <c r="A90" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C90" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D90" s="15" t="s">
+      <c r="D90" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E90" s="15" t="s">
+      <c r="E90" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F90" s="15" t="s">
+      <c r="F90" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G90" s="15" t="s">
+      <c r="G90" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33599,22 +33616,22 @@
       <c r="A91" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C91" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E91" s="15" t="s">
+      <c r="E91" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F91" s="15" t="s">
+      <c r="F91" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G91" s="15" t="s">
+      <c r="G91" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33622,22 +33639,22 @@
       <c r="A92" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C92" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E92" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F92" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E92" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F92" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G92" s="15" t="s">
+      <c r="G92" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33645,22 +33662,22 @@
       <c r="A93" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C93" s="1" t="s">
+      <c r="C93" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E93" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F93" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E93" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F93" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G93" s="15" t="s">
+      <c r="G93" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33668,22 +33685,22 @@
       <c r="A94" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C94" s="1" t="s">
+      <c r="C94" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="D94" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E94" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F94" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E94" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F94" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G94" s="15" t="s">
+      <c r="G94" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33691,22 +33708,22 @@
       <c r="A95" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D95" s="15" t="s">
+      <c r="D95" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E95" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F95" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E95" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F95" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G95" s="15" t="s">
+      <c r="G95" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33714,22 +33731,22 @@
       <c r="A96" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C96" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D96" s="15" t="s">
+      <c r="D96" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E96" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F96" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E96" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F96" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G96" s="15" t="s">
+      <c r="G96" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33737,22 +33754,22 @@
       <c r="A97" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D97" s="15" t="s">
+      <c r="C97" s="15" t="s">
+        <v>578</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E97" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="F97" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E97" s="15" t="s">
-        <v>572</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G97" s="15" t="s">
+      <c r="G97" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33760,22 +33777,22 @@
       <c r="A98" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C98" s="1" t="s">
+      <c r="C98" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D98" s="15" t="s">
+      <c r="D98" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E98" s="15" t="s">
+      <c r="E98" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F98" s="15" t="s">
+      <c r="F98" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G98" s="15" t="s">
+      <c r="G98" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33783,22 +33800,22 @@
       <c r="A99" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C99" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D99" s="15" t="s">
+      <c r="D99" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E99" s="15" t="s">
+      <c r="E99" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F99" s="15" t="s">
+      <c r="F99" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G99" s="15" t="s">
+      <c r="G99" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33806,22 +33823,22 @@
       <c r="A100" s="12" t="s">
         <v>410</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C100" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D100" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E100" s="15" t="s">
+      <c r="D100" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E100" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F100" s="15" t="s">
+      <c r="F100" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G100" s="15" t="s">
+      <c r="G100" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33829,22 +33846,22 @@
       <c r="A101" s="12" t="s">
         <v>411</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C101" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D101" s="15" t="s">
+      <c r="D101" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E101" s="15" t="s">
+      <c r="E101" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F101" s="15" t="s">
+      <c r="F101" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G101" s="15" t="s">
+      <c r="G101" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33852,22 +33869,22 @@
       <c r="A102" s="12" t="s">
         <v>417</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C102" s="1" t="s">
+      <c r="C102" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E102" s="15" t="s">
+      <c r="E102" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F102" s="15" t="s">
+      <c r="F102" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G102" s="15" t="s">
+      <c r="G102" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33875,22 +33892,22 @@
       <c r="A103" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D103" s="15" t="s">
+      <c r="D103" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E103" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E103" s="15" t="s">
+      <c r="F103" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F103" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G103" s="15" t="s">
+      <c r="G103" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -33898,22 +33915,22 @@
       <c r="A104" s="12" t="s">
         <v>425</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D104" s="15" t="s">
+      <c r="D104" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E104" s="15" t="s">
+      <c r="E104" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F104" s="15" t="s">
+      <c r="F104" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G104" s="15" t="s">
+      <c r="G104" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33921,22 +33938,22 @@
       <c r="A105" s="12" t="s">
         <v>426</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C105" s="1" t="s">
+      <c r="C105" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D105" s="15" t="s">
+      <c r="D105" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E105" s="15" t="s">
+      <c r="E105" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F105" s="15" t="s">
+      <c r="F105" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G105" s="15" t="s">
+      <c r="G105" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33944,22 +33961,22 @@
       <c r="A106" s="12" t="s">
         <v>430</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C106" s="1" t="s">
+      <c r="C106" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D106" s="15" t="s">
+      <c r="D106" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F106" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E106" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F106" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G106" s="15" t="s">
+      <c r="G106" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33967,22 +33984,22 @@
       <c r="A107" s="12" t="s">
         <v>435</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D107" s="15" t="s">
+      <c r="D107" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F107" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E107" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F107" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G107" s="15" t="s">
+      <c r="G107" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -33990,22 +34007,22 @@
       <c r="A108" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D108" s="15" t="s">
+      <c r="D108" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E108" s="15" t="s">
+      <c r="E108" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F108" s="15" t="s">
+      <c r="F108" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G108" s="15" t="s">
+      <c r="G108" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34013,22 +34030,22 @@
       <c r="A109" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D109" s="15" t="s">
+      <c r="D109" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E109" s="15" t="s">
+      <c r="E109" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F109" s="15" t="s">
+      <c r="F109" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G109" s="15" t="s">
+      <c r="G109" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34036,22 +34053,22 @@
       <c r="A110" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C110" s="1" t="s">
+      <c r="C110" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D110" s="15" t="s">
+      <c r="D110" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E110" s="15" t="s">
+      <c r="E110" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F110" s="15" t="s">
+      <c r="F110" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G110" s="15" t="s">
+      <c r="G110" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34059,22 +34076,22 @@
       <c r="A111" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C111" s="1" t="s">
+      <c r="C111" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D111" s="15" t="s">
+      <c r="D111" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E111" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E111" s="15" t="s">
+      <c r="F111" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F111" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G111" s="15" t="s">
+      <c r="G111" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34082,22 +34099,22 @@
       <c r="A112" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C112" s="1" t="s">
+      <c r="C112" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D112" s="15" t="s">
+      <c r="D112" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F112" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E112" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F112" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G112" s="15" t="s">
+      <c r="G112" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34105,22 +34122,22 @@
       <c r="A113" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C113" s="1" t="s">
+      <c r="C113" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D113" s="15" t="s">
+      <c r="D113" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="F113" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E113" s="15" t="s">
-        <v>567</v>
-      </c>
-      <c r="F113" s="15" t="s">
-        <v>566</v>
-      </c>
-      <c r="G113" s="15" t="s">
+      <c r="G113" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34128,22 +34145,22 @@
       <c r="A114" s="12" t="s">
         <v>459</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C114" s="1" t="s">
+      <c r="C114" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D114" s="15" t="s">
+      <c r="D114" s="16" t="s">
         <v>574</v>
       </c>
-      <c r="E114" s="15" t="s">
+      <c r="E114" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F114" s="15" t="s">
+      <c r="F114" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G114" s="15" t="s">
+      <c r="G114" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34151,22 +34168,22 @@
       <c r="A115" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C115" s="1" t="s">
+      <c r="C115" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D115" s="15" t="s">
+      <c r="D115" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E115" s="15" t="s">
+      <c r="E115" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F115" s="15" t="s">
+      <c r="F115" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G115" s="15" t="s">
+      <c r="G115" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34174,22 +34191,22 @@
       <c r="A116" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D116" s="15" t="s">
+      <c r="D116" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E116" s="15" t="s">
+      <c r="E116" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="F116" s="15" t="s">
+      <c r="F116" s="16" t="s">
         <v>571</v>
       </c>
-      <c r="G116" s="15" t="s">
+      <c r="G116" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34197,45 +34214,45 @@
       <c r="A117" s="12" t="s">
         <v>468</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D117" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="E117" s="15" t="s">
+      <c r="D117" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="E117" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F117" s="15" t="s">
+      <c r="F117" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G117" s="15" t="s">
+      <c r="G117" s="16" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="12" t="s">
-        <v>578</v>
-      </c>
-      <c r="B118" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B118" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C118" s="1" t="s">
+      <c r="C118" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D118" s="15" t="s">
+      <c r="D118" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E118" s="15" t="s">
+      <c r="E118" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F118" s="15" t="s">
+      <c r="F118" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G118" s="15" t="s">
+      <c r="G118" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34243,22 +34260,22 @@
       <c r="A119" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C119" s="1" t="s">
+      <c r="C119" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D119" s="15" t="s">
+      <c r="D119" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E119" s="15" t="s">
+      <c r="E119" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F119" s="15" t="s">
+      <c r="F119" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G119" s="15" t="s">
+      <c r="G119" s="16" t="s">
         <v>568</v>
       </c>
     </row>
@@ -34266,22 +34283,22 @@
       <c r="A120" s="12" t="s">
         <v>472</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="C120" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D120" s="15" t="s">
+      <c r="D120" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="E120" s="15" t="s">
+      <c r="E120" s="16" t="s">
         <v>567</v>
       </c>
-      <c r="F120" s="15" t="s">
+      <c r="F120" s="16" t="s">
         <v>566</v>
       </c>
-      <c r="G120" s="15" t="s">
+      <c r="G120" s="16" t="s">
         <v>569</v>
       </c>
     </row>
@@ -34289,22 +34306,22 @@
       <c r="A121" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="C121" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D121" s="15" t="s">
+      <c r="D121" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E121" s="15" t="s">
+      <c r="E121" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F121" s="15" t="s">
+      <c r="F121" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G121" s="15" t="s">
+      <c r="G121" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34312,22 +34329,22 @@
       <c r="A122" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D122" s="15" t="s">
+      <c r="D122" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E122" s="15" t="s">
+      <c r="E122" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F122" s="15" t="s">
+      <c r="F122" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G122" s="15" t="s">
+      <c r="G122" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34335,22 +34352,22 @@
       <c r="A123" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="C123" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D123" s="15" t="s">
+      <c r="D123" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E123" s="15" t="s">
+      <c r="E123" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F123" s="15" t="s">
+      <c r="F123" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G123" s="15" t="s">
+      <c r="G123" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34358,22 +34375,22 @@
       <c r="A124" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="C124" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D124" s="15" t="s">
+      <c r="D124" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E124" s="15" t="s">
+      <c r="E124" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F124" s="15" t="s">
+      <c r="F124" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G124" s="15" t="s">
+      <c r="G124" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34381,22 +34398,22 @@
       <c r="A125" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D125" s="15" t="s">
+      <c r="D125" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E125" s="15" t="s">
+      <c r="E125" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F125" s="15" t="s">
+      <c r="F125" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G125" s="15" t="s">
+      <c r="G125" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34404,22 +34421,22 @@
       <c r="A126" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C126" s="1" t="s">
+      <c r="C126" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D126" s="15" t="s">
+      <c r="D126" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E126" s="15" t="s">
+      <c r="E126" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F126" s="15" t="s">
+      <c r="F126" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G126" s="15" t="s">
+      <c r="G126" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34427,22 +34444,22 @@
       <c r="A127" s="12" t="s">
         <v>499</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C127" s="1" t="s">
+      <c r="C127" s="15" t="s">
         <v>565</v>
       </c>
-      <c r="D127" s="15" t="s">
+      <c r="D127" s="16" t="s">
         <v>572</v>
       </c>
-      <c r="E127" s="15" t="s">
+      <c r="E127" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F127" s="15" t="s">
+      <c r="F127" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="G127" s="15" t="s">
+      <c r="G127" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34450,22 +34467,22 @@
       <c r="A128" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="C128" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D128" s="15" t="s">
+      <c r="D128" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E128" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E128" s="15" t="s">
+      <c r="F128" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F128" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G128" s="15" t="s">
+      <c r="G128" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34473,22 +34490,22 @@
       <c r="A129" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="C129" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D129" s="15" t="s">
+      <c r="D129" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E129" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E129" s="15" t="s">
+      <c r="F129" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F129" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G129" s="15" t="s">
+      <c r="G129" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34496,22 +34513,22 @@
       <c r="A130" s="12" t="s">
         <v>507</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D130" s="15" t="s">
+      <c r="D130" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E130" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E130" s="15" t="s">
+      <c r="F130" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F130" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G130" s="15" t="s">
+      <c r="G130" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34519,22 +34536,22 @@
       <c r="A131" s="12" t="s">
         <v>509</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="C131" s="1" t="s">
+      <c r="C131" s="15" t="s">
         <v>570</v>
       </c>
-      <c r="D131" s="15" t="s">
+      <c r="D131" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E131" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E131" s="15" t="s">
+      <c r="F131" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F131" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G131" s="15" t="s">
+      <c r="G131" s="16" t="s">
         <v>570</v>
       </c>
     </row>
@@ -34542,29 +34559,26 @@
       <c r="A132" s="14" t="s">
         <v>512</v>
       </c>
-      <c r="B132" s="15" t="s">
+      <c r="B132" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="C132" s="15" t="s">
+      <c r="C132" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="D132" s="15" t="s">
+      <c r="D132" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="E132" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="E132" s="15" t="s">
+      <c r="F132" s="16" t="s">
         <v>570</v>
       </c>
-      <c r="F132" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="G132" s="15" t="s">
+      <c r="G132" s="16" t="s">
         <v>570</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://doi.org/10.1016/j.humimm.2007.01.014"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>